<commit_message>
EPBDS-7984 Copy() functionality doesn't work with Array parameters in Spreadsheets
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7984_Copy.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7984_Copy.xlsx
@@ -4,87 +4,170 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="10290" windowWidth="23955" xWindow="360" yWindow="105"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="23955" windowHeight="10290"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="Copy" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
-  <si>
-    <t>Spreadsheet SpreadsheetResult mySpr3(Integer[] a)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Steps</t>
   </si>
   <si>
-    <t>myValue</t>
-  </si>
-  <si>
-    <t>myValuecopy</t>
-  </si>
-  <si>
-    <t>= a</t>
-  </si>
-  <si>
-    <t>=copy($myValue)</t>
-  </si>
-  <si>
-    <t>Spreadsheet SpreadsheetResult mySpr4(Integer[] a)</t>
-  </si>
-  <si>
     <t>=a</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Test mySpr3 mySpr3Test</t>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>copied</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>= sum ($copied)</t>
+  </si>
+  <si>
+    <t>originSum</t>
+  </si>
+  <si>
+    <t>= sum ($origin)</t>
+  </si>
+  <si>
+    <t>equals</t>
+  </si>
+  <si>
+    <t>= $copied == $origin</t>
+  </si>
+  <si>
+    <t>equalsSum</t>
+  </si>
+  <si>
+    <t>= $sum == $originSum</t>
+  </si>
+  <si>
+    <t>equalsOrigin</t>
+  </si>
+  <si>
+    <t>= a == $origin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">= a == $copied </t>
+  </si>
+  <si>
+    <t>equalsCopied</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult epbds_7984(Integer[] a)</t>
+  </si>
+  <si>
+    <t>Test epbds_7984</t>
+  </si>
+  <si>
+    <t>#1</t>
+  </si>
+  <si>
+    <t>#2</t>
+  </si>
+  <si>
+    <t>#3</t>
   </si>
   <si>
     <t>a</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>_res_</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t>_res_.myValuecopy</t>
-  </si>
-  <si>
-    <t>_res_.$Value$myValuecopy</t>
+    <t>Calc</t>
+  </si>
+  <si>
+    <t>_res_.$Calc$origin</t>
+  </si>
+  <si>
+    <t>1,,3</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>_res_.$Calc$copied</t>
+  </si>
+  <si>
+    <t>_res_.$Calc$sum</t>
+  </si>
+  <si>
+    <t>_res_.$Calc$originSum</t>
+  </si>
+  <si>
+    <t>_res_.$Calc$equals</t>
+  </si>
+  <si>
+    <t>_res_.$Calc$equalsSum</t>
+  </si>
+  <si>
+    <t>_res_.$Calc$equalsOrigin</t>
+  </si>
+  <si>
+    <t>_res_.$Calc$equalsCopied</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Array</t>
+  </si>
+  <si>
+    <t>Origin</t>
+  </si>
+  <si>
+    <t>Copied</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Origin Sum</t>
+  </si>
+  <si>
+    <t>a == copy</t>
+  </si>
+  <si>
+    <t>a == origin</t>
+  </si>
+  <si>
+    <t>copied == origin</t>
+  </si>
+  <si>
+    <t>sum == originSum</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>_id_</t>
+  </si>
+  <si>
+    <t>=copy ($origin)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="000000" theme="1"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,7 +178,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -103,36 +186,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -158,10 +225,10 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2">
-    <tableStyle count="2" name="MySqlDefault" pivot="0" table="0">
-      <tableStyleElement dxfId="1" type="wholeTable"/>
-      <tableStyleElement dxfId="0" type="headerRow"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -177,10 +244,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -338,7 +405,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -347,13 +414,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -363,7 +430,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -372,7 +439,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -381,7 +448,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -391,12 +458,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -427,7 +494,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -446,7 +513,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -458,109 +525,278 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:C19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="45.28515625" collapsed="true"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="44.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="E5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
       <c r="C6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25"/>
-    <row r="16">
-      <c r="B16" s="3" t="s">
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>6</v>
+      </c>
+      <c r="I9" s="1">
+        <v>4</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>6</v>
+      </c>
+      <c r="I10" s="1">
+        <v>4</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17">
-      <c r="B17" t="s" s="3">
+      <c r="E13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="s" s="3">
+      <c r="C14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C18" t="s" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>14</v>
+      <c r="E14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells>
-    <mergeCell ref="B16:C16"/>
+  <mergeCells count="1">
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>